<commit_message>
actualización del plan de la configuracion, cronograma, product backlog y subiendo el informe y el acta del ultimo sprint
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDC/Documentos/DocumentosSprint/SGDC_SB2_1.1.xlsx
+++ b/Desarrollo/SGDC/Documentos/DocumentosSprint/SGDC_SB2_1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNMSM_Cursos\fisi_8vo_ciclo\Gest_conf_mantto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fisi_UNMSM\fisi_8vo_ciclo\Gest_conf_mantto\HernandezLivia\CodeMentorSolutions\Desarrollo\SGDC\Documentos\DocumentosSprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -405,104 +405,104 @@
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,10 +722,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:AI15"/>
+  <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -743,252 +743,252 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="29">
         <v>2</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="32" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="32" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
     </row>
     <row r="9" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="19" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="15" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17" t="s">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="2:10" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="23" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>